<commit_message>
direction switcher : started
</commit_message>
<xml_diff>
--- a/Test documents/Return Report COD/output.xlsx
+++ b/Test documents/Return Report COD/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ecommerce-Automation\Test documents\Return Report COD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2539C7-69D7-4BFC-B275-3429CA1C1D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF18595F-5179-43CB-A601-DFBC6265767D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1142,7 +1142,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomLeft" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>